<commit_message>
updating script and output to incorporate new ViewTaxonomy file from ForestGEO.
</commit_message>
<xml_diff>
--- a/tocheck/Perezlistnombrenoacceptado.xlsx
+++ b/tocheck/Perezlistnombrenoacceptado.xlsx
@@ -522,6 +522,11 @@
           <t>Citrus aurantium</t>
         </is>
       </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>citrsi</t>
+        </is>
+      </c>
       <c r="M2" t="inlineStr">
         <is>
           <t>citrsi</t>
@@ -558,7 +563,7 @@
         </is>
       </c>
       <c r="T2" s="2">
-        <v>45909</v>
+        <v>45979</v>
       </c>
       <c r="U2" t="b">
         <v>0</v>
@@ -651,7 +656,7 @@
         </is>
       </c>
       <c r="T3" s="2">
-        <v>45909</v>
+        <v>45979</v>
       </c>
       <c r="U3" t="b">
         <v>0</v>
@@ -739,7 +744,7 @@
         </is>
       </c>
       <c r="T4" s="2">
-        <v>45909</v>
+        <v>45979</v>
       </c>
       <c r="U4" t="b">
         <v>0</v>
@@ -837,7 +842,7 @@
         </is>
       </c>
       <c r="T5" s="2">
-        <v>45909</v>
+        <v>45979</v>
       </c>
       <c r="U5" t="b">
         <v>0</v>
@@ -920,7 +925,7 @@
         </is>
       </c>
       <c r="T6" s="2">
-        <v>45909</v>
+        <v>45979</v>
       </c>
       <c r="U6" t="b">
         <v>0</v>
@@ -1008,7 +1013,7 @@
         </is>
       </c>
       <c r="T7" s="2">
-        <v>45909</v>
+        <v>45979</v>
       </c>
       <c r="U7" t="b">
         <v>0</v>
@@ -1106,7 +1111,7 @@
         </is>
       </c>
       <c r="T8" s="2">
-        <v>45909</v>
+        <v>45979</v>
       </c>
       <c r="U8" t="b">
         <v>0</v>
@@ -1209,7 +1214,7 @@
         </is>
       </c>
       <c r="T9" s="2">
-        <v>45909</v>
+        <v>45979</v>
       </c>
       <c r="U9" t="b">
         <v>0</v>
@@ -1297,7 +1302,7 @@
         </is>
       </c>
       <c r="T10" s="2">
-        <v>45909</v>
+        <v>45979</v>
       </c>
       <c r="U10" t="b">
         <v>0</v>
@@ -1385,7 +1390,7 @@
         </is>
       </c>
       <c r="T11" s="2">
-        <v>45909</v>
+        <v>45979</v>
       </c>
       <c r="U11" t="b">
         <v>0</v>

</xml_diff>